<commit_message>
fix: Excel Change Management jetzt als Prozentsatz, H2 Spacing korrigiert
- Excel: Change Management wird nun als 12% der Basiskosten berechnet
  (entspricht Artikel-Angabe "10-15% der Gesamtkosten")
- CSS: H2 Überschriften bekommen jetzt konsistent dreifachen Abstand
  vorher (9rem) und doppelten Abstand danach (4rem)
- !important überschreibt Inline-Tailwind-Klassen wie mb-6

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/downloads/Copilot-ROI-Rechner.xlsx
+++ b/public/downloads/Copilot-ROI-Rechner.xlsx
@@ -179,13 +179,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -193,8 +193,8 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -795,27 +795,27 @@
       </c>
       <c r="D15" s="7" t="inlineStr">
         <is>
-          <t>Integration, Rollout</t>
+          <t>Integration, Rollout (€10k-50k)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="inlineStr">
         <is>
-          <t>Change Management (einmalig)</t>
-        </is>
-      </c>
-      <c r="B16" s="8" t="n">
-        <v>15000</v>
+          <t>Change Management</t>
+        </is>
+      </c>
+      <c r="B16" s="9" t="n">
+        <v>0.12</v>
       </c>
       <c r="C16" s="7" t="inlineStr">
         <is>
-          <t>€</t>
+          <t>% der Basiskosten</t>
         </is>
       </c>
       <c r="D16" s="7" t="inlineStr">
         <is>
-          <t>Kommunikation, Support</t>
+          <t>Artikel empfiehlt: 10-15%</t>
         </is>
       </c>
     </row>
@@ -874,12 +874,12 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="inlineStr">
+      <c r="A21" s="10" t="inlineStr">
         <is>
           <t>→ Erwartete Adoption-Rate</t>
         </is>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="11">
         <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-B20/600))))</f>
         <v/>
       </c>
@@ -895,28 +895,28 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11" t="inlineStr">
+      <c r="A23" s="12" t="inlineStr">
         <is>
           <t>Hinweis zur Adoption-Rate:</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="13" t="inlineStr">
         <is>
           <t>Die Adoption-Rate zeigt, wie viele Mitarbeiter Copilot regelmäßig nutzen.</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="inlineStr">
+      <c r="A25" s="13" t="inlineStr">
         <is>
           <t>Ohne gezieltes Training liegt diese erfahrungsgemäß bei nur 5-15%.</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12" t="inlineStr">
+      <c r="A26" s="13" t="inlineStr">
         <is>
           <t>Mit professionellem Training (€800-1.500/MA) erreichen Sie 60-85% Adoption.</t>
         </is>
@@ -962,7 +962,7 @@
           <t>Zeitersparnis pro aktivem Nutzer</t>
         </is>
       </c>
-      <c r="B30" s="13" t="n">
+      <c r="B30" s="9" t="n">
         <v>0.25</v>
       </c>
       <c r="C30" s="7" t="inlineStr">
@@ -1021,7 +1021,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,9 +1071,10 @@
           <t>Lizenzen (12 Monate)</t>
         </is>
       </c>
-      <c r="B4" s="7">
-        <f>CONCATENATE('1. Eingaben'!B7," × €",'1. Eingaben'!B14," × 12")</f>
-        <v/>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>Nutzer × €30 × 12</t>
+        </is>
       </c>
       <c r="C4" s="16">
         <f>'1. Eingaben'!B7*'1. Eingaben'!B14*12</f>
@@ -1090,9 +1091,10 @@
           <t>Training &amp; Schulung</t>
         </is>
       </c>
-      <c r="B5" s="7">
-        <f>CONCATENATE('1. Eingaben'!B7," × €",'1. Eingaben'!B20)</f>
-        <v/>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Nutzer × Training-Budget</t>
+        </is>
       </c>
       <c r="C5" s="16">
         <f>'1. Eingaben'!B7*'1. Eingaben'!B20</f>
@@ -1124,16 +1126,16 @@
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>Change Management</t>
+          <t>Change Management (10-15%)</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>Einmalig</t>
+          <t>% der Basiskosten</t>
         </is>
       </c>
       <c r="C7" s="16">
-        <f>'1. Eingaben'!B16</f>
+        <f>'1. Eingaben'!B16*(C4+C5+C6)</f>
         <v/>
       </c>
       <c r="D7" s="16" t="n">
@@ -1162,13 +1164,24 @@
           <t>Anteil Training an Gesamtkosten Jahr 1</t>
         </is>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="11">
         <f>C5/C9</f>
         <v/>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="14" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>Change Management Betrag</t>
+        </is>
+      </c>
+      <c r="C12" s="19">
+        <f>C7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="14" t="inlineStr">
         <is>
           <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot</t>
         </is>
@@ -1225,7 +1238,7 @@
           <t>Arbeitszeit pro Nutzer/Jahr (Stunden)</t>
         </is>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="20">
         <f>'1. Eingaben'!B9*'1. Eingaben'!B10</f>
         <v/>
       </c>
@@ -1236,7 +1249,7 @@
           <t>Gesamtarbeitszeit alle Nutzer (Stunden)</t>
         </is>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="20">
         <f>B5*'1. Eingaben'!B7</f>
         <v/>
       </c>
@@ -1247,7 +1260,7 @@
           <t>Stundensatz</t>
         </is>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <f>'1. Eingaben'!B8</f>
         <v/>
       </c>
@@ -1258,7 +1271,7 @@
           <t>Adoption-Rate (aus Training)</t>
         </is>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="11">
         <f>'1. Eingaben'!B21</f>
         <v/>
       </c>
@@ -1269,7 +1282,7 @@
           <t>Zeitersparnis pro aktivem Nutzer</t>
         </is>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="11">
         <f>'1. Eingaben'!B30</f>
         <v/>
       </c>
@@ -2000,7 +2013,7 @@
     <row r="16">
       <c r="A16" s="7" t="inlineStr">
         <is>
-          <t>Break-even</t>
+          <t>Break-even (Monate)</t>
         </is>
       </c>
       <c r="B16" s="25">

</xml_diff>

<commit_message>
feat: Studiendaten integriert - Forrester 9h/Monat, Work Trend Index 77%
</commit_message>
<xml_diff>
--- a/public/downloads/Copilot-ROI-Rechner.xlsx
+++ b/public/downloads/Copilot-ROI-Rechner.xlsx
@@ -25,7 +25,7 @@
     <numFmt numFmtId="165" formatCode="+#,##0 €;-#,##0 €"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,6 +45,14 @@
     <font>
       <b val="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="001F4E79"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="9"/>
     </font>
     <font>
       <b val="1"/>
@@ -71,6 +79,11 @@
       <color rgb="00375623"/>
     </font>
     <font>
+      <i val="1"/>
+      <color rgb="00666666"/>
+      <sz val="9"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
     <font>
@@ -79,12 +92,10 @@
       <sz val="18"/>
     </font>
     <font>
-      <i val="1"/>
-      <color rgb="00666666"/>
-      <sz val="9"/>
+      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -94,6 +105,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00D6DCE5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8F4FD"/>
       </patternFill>
     </fill>
     <fill>
@@ -163,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -172,51 +188,58 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="11" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -582,7 +605,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,10 +613,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="38" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
     <col width="5" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -614,7 +637,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>UNTERNEHMENSDATEN</t>
+          <t>STUDIENERGEBNISSE (REFERENZWERTE)</t>
         </is>
       </c>
       <c r="B5" s="4" t="n"/>
@@ -625,391 +648,397 @@
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
+          <t>Zeitersparnis pro Nutzer/Monat</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>9 Stunden</t>
+        </is>
+      </c>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>Quelle: Forrester TEI Study</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Produktivitätssteigerung (trainierte Nutzer)</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>77%</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>Quelle: Microsoft Work Trend Index</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>UNTERNEHMENSDATEN</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="4" t="n"/>
+      <c r="E10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="inlineStr">
+        <is>
           <t>Parameter</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B11" s="9" t="inlineStr">
         <is>
           <t>Wert</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C11" s="9" t="inlineStr">
         <is>
           <t>Einheit</t>
         </is>
       </c>
-      <c r="D6" s="6" t="inlineStr">
+      <c r="D11" s="9" t="inlineStr">
         <is>
           <t>Hinweis</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="E11" s="9" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Anzahl Copilot-Nutzer</t>
         </is>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B12" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C12" s="10" t="inlineStr">
         <is>
           <t>Mitarbeiter</t>
         </is>
       </c>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="D12" s="10" t="inlineStr">
         <is>
           <t>Geplante Lizenzen</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="7" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>Durchschnittlicher Stundensatz</t>
         </is>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B13" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="C8" s="7" t="inlineStr">
+      <c r="C13" s="10" t="inlineStr">
         <is>
           <t>€/Stunde</t>
         </is>
       </c>
-      <c r="D8" s="7" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>Vollkosten inkl. Nebenkosten</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="7" t="inlineStr">
-        <is>
-          <t>Arbeitsstunden pro Woche</t>
-        </is>
-      </c>
-      <c r="B9" s="8" t="n">
-        <v>40</v>
-      </c>
-      <c r="C9" s="7" t="inlineStr">
-        <is>
-          <t>Stunden</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr">
-        <is>
-          <t>Standard: 40</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="inlineStr">
-        <is>
-          <t>Arbeitswochen pro Jahr</t>
-        </is>
-      </c>
-      <c r="B10" s="8" t="n">
-        <v>48</v>
-      </c>
-      <c r="C10" s="7" t="inlineStr">
-        <is>
-          <t>Wochen</t>
-        </is>
-      </c>
-      <c r="D10" s="7" t="inlineStr">
-        <is>
-          <t>Abzgl. Urlaub/Feiertage</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>LIZENZKOSTEN</t>
         </is>
       </c>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="5" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="inlineStr">
+      <c r="B15" s="4" t="n"/>
+      <c r="C15" s="4" t="n"/>
+      <c r="D15" s="4" t="n"/>
+      <c r="E15" s="5" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="9" t="inlineStr">
         <is>
           <t>Parameter</t>
         </is>
       </c>
-      <c r="B13" s="6" t="inlineStr">
+      <c r="B16" s="9" t="inlineStr">
         <is>
           <t>Wert</t>
         </is>
       </c>
-      <c r="C13" s="6" t="inlineStr">
+      <c r="C16" s="9" t="inlineStr">
         <is>
           <t>Einheit</t>
         </is>
       </c>
-      <c r="D13" s="6" t="inlineStr">
+      <c r="D16" s="9" t="inlineStr">
         <is>
           <t>Hinweis</t>
         </is>
       </c>
-      <c r="E13" s="6" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="E16" s="9" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>Copilot Lizenzkosten pro Monat</t>
         </is>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B17" s="11" t="n">
         <v>30</v>
       </c>
-      <c r="C14" s="7" t="inlineStr">
+      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>€/Nutzer</t>
         </is>
       </c>
-      <c r="D14" s="7" t="inlineStr">
+      <c r="D17" s="10" t="inlineStr">
         <is>
           <t>M365 Copilot: €30</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>IT-Setup (einmalig)</t>
         </is>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B18" s="11" t="n">
         <v>25000</v>
       </c>
-      <c r="C15" s="7" t="inlineStr">
+      <c r="C18" s="10" t="inlineStr">
         <is>
           <t>€</t>
         </is>
       </c>
-      <c r="D15" s="7" t="inlineStr">
+      <c r="D18" s="10" t="inlineStr">
         <is>
           <t>Integration, Rollout (€10k-50k)</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="7" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>Change Management</t>
         </is>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B19" s="12" t="n">
         <v>0.12</v>
       </c>
-      <c r="C16" s="7" t="inlineStr">
+      <c r="C19" s="10" t="inlineStr">
         <is>
           <t>% der Basiskosten</t>
         </is>
       </c>
-      <c r="D16" s="7" t="inlineStr">
-        <is>
-          <t>Artikel empfiehlt: 10-15%</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="D19" s="10" t="inlineStr">
+        <is>
+          <t>Empfohlen: 10-15%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>TRAINING &amp; ENABLEMENT</t>
         </is>
       </c>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="5" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
+      <c r="B21" s="4" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="4" t="n"/>
+      <c r="E21" s="5" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="inlineStr">
         <is>
           <t>Parameter</t>
         </is>
       </c>
-      <c r="B19" s="6" t="inlineStr">
+      <c r="B22" s="9" t="inlineStr">
         <is>
           <t>Wert</t>
         </is>
       </c>
-      <c r="C19" s="6" t="inlineStr">
+      <c r="C22" s="9" t="inlineStr">
         <is>
           <t>Einheit</t>
         </is>
       </c>
-      <c r="D19" s="6" t="inlineStr">
+      <c r="D22" s="9" t="inlineStr">
         <is>
           <t>Hinweis</t>
         </is>
       </c>
-      <c r="E19" s="6" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="7" t="inlineStr">
+      <c r="E22" s="9" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="inlineStr">
         <is>
           <t>Training-Budget pro Mitarbeiter</t>
         </is>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B23" s="11" t="n">
         <v>800</v>
       </c>
-      <c r="C20" s="7" t="inlineStr">
+      <c r="C23" s="10" t="inlineStr">
         <is>
           <t>€/Mitarbeiter</t>
         </is>
       </c>
-      <c r="D20" s="7" t="inlineStr">
+      <c r="D23" s="10" t="inlineStr">
         <is>
           <t>Empfohlen: €500-1.500</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="10" t="inlineStr">
-        <is>
-          <t>→ Erwartete Adoption-Rate</t>
-        </is>
-      </c>
-      <c r="B21" s="11">
-        <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-B20/600))))</f>
-        <v/>
-      </c>
-      <c r="C21" s="7" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D21" s="7" t="inlineStr">
-        <is>
-          <t>Berechnet aus Training-Budget</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="12" t="inlineStr">
-        <is>
-          <t>Hinweis zur Adoption-Rate:</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="inlineStr">
         <is>
-          <t>Die Adoption-Rate zeigt, wie viele Mitarbeiter Copilot regelmäßig nutzen.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="13" t="inlineStr">
-        <is>
-          <t>Ohne gezieltes Training liegt diese erfahrungsgemäß bei nur 5-15%.</t>
+          <t>→ Erwartete Adoption-Rate</t>
+        </is>
+      </c>
+      <c r="B24" s="14">
+        <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-B23/600))))</f>
+        <v/>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D24" s="10" t="inlineStr">
+        <is>
+          <t>Berechnet aus Training-Budget</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="inlineStr">
+      <c r="A26" s="15" t="inlineStr">
+        <is>
+          <t>Hinweis zur Adoption-Rate (basierend auf Work Trend Index):</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="16" t="inlineStr">
+        <is>
+          <t>77% der trainierten Nutzer berichten höhere Produktivität.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="16" t="inlineStr">
+        <is>
+          <t>Ohne gezieltes Training liegt die aktive Nutzung oft bei nur 5-15%.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="16" t="inlineStr">
         <is>
           <t>Mit professionellem Training (€800-1.500/MA) erreichen Sie 60-85% Adoption.</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="3" t="inlineStr">
-        <is>
-          <t>PRODUKTIVITÄTSANNAHMEN</t>
-        </is>
-      </c>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="n"/>
-      <c r="E28" s="5" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="6" t="inlineStr">
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>PRODUKTIVITÄTSANNAHMEN (FORRESTER TEI STUDY)</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="4" t="n"/>
+      <c r="E31" s="5" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="9" t="inlineStr">
         <is>
           <t>Parameter</t>
         </is>
       </c>
-      <c r="B29" s="6" t="inlineStr">
+      <c r="B32" s="9" t="inlineStr">
         <is>
           <t>Wert</t>
         </is>
       </c>
-      <c r="C29" s="6" t="inlineStr">
+      <c r="C32" s="9" t="inlineStr">
         <is>
           <t>Einheit</t>
         </is>
       </c>
-      <c r="D29" s="6" t="inlineStr">
+      <c r="D32" s="9" t="inlineStr">
         <is>
           <t>Hinweis</t>
         </is>
       </c>
-      <c r="E29" s="6" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="7" t="inlineStr">
+      <c r="E32" s="9" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="inlineStr">
         <is>
           <t>Zeitersparnis pro aktivem Nutzer</t>
         </is>
       </c>
-      <c r="B30" s="9" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C30" s="7" t="inlineStr">
-        <is>
-          <t>% der Arbeitszeit</t>
-        </is>
-      </c>
-      <c r="D30" s="7" t="inlineStr">
-        <is>
-          <t>Studien zeigen: 20-30%</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="7" t="inlineStr">
+      <c r="B33" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>Stunden/Monat</t>
+        </is>
+      </c>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t>Forrester TEI: 9h/Monat</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="10" t="inlineStr">
         <is>
           <t>Lernkurve (Monate bis Vollnutzung)</t>
         </is>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B34" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="7" t="inlineStr">
+      <c r="C34" s="10" t="inlineStr">
         <is>
           <t>Monate</t>
         </is>
       </c>
-      <c r="D31" s="7" t="inlineStr">
+      <c r="D34" s="10" t="inlineStr">
         <is>
           <t>Mit Training: 2-3, ohne: 6-12</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="14" t="inlineStr">
-        <is>
-          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot</t>
+    <row r="37">
+      <c r="A37" s="17" t="inlineStr">
+        <is>
+          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot | Datenquellen: Forrester TEI, Microsoft Work Trend Index</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A28:E28"/>
+  <mergeCells count="6">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A10:E10"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A31:E31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1021,7 +1050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,167 +1058,177 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="32" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>KOSTENKALKULATION</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>Kostenart</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
           <t>Berechnung</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" s="9" t="inlineStr">
         <is>
           <t>Jahr 1 (€)</t>
         </is>
       </c>
-      <c r="D3" s="6" t="inlineStr">
+      <c r="D3" s="9" t="inlineStr">
         <is>
           <t>Jahre 2-5 (€/Jahr)</t>
         </is>
       </c>
-      <c r="E3" s="6" t="inlineStr"/>
+      <c r="E3" s="9" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>Lizenzen (12 Monate)</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>Nutzer × €30 × 12</t>
         </is>
       </c>
-      <c r="C4" s="16">
-        <f>'1. Eingaben'!B7*'1. Eingaben'!B14*12</f>
-        <v/>
-      </c>
-      <c r="D4" s="16">
-        <f>'1. Eingaben'!B7*'1. Eingaben'!B14*12</f>
+      <c r="C4" s="19">
+        <f>'1. Eingaben'!B12*'1. Eingaben'!B17*12</f>
+        <v/>
+      </c>
+      <c r="D4" s="19">
+        <f>'1. Eingaben'!B12*'1. Eingaben'!B17*12</f>
         <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Training &amp; Schulung</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Nutzer × Training-Budget</t>
         </is>
       </c>
-      <c r="C5" s="16">
-        <f>'1. Eingaben'!B7*'1. Eingaben'!B20</f>
-        <v/>
-      </c>
-      <c r="D5" s="16" t="n">
+      <c r="C5" s="19">
+        <f>'1. Eingaben'!B12*'1. Eingaben'!B23</f>
+        <v/>
+      </c>
+      <c r="D5" s="19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>IT-Setup &amp; Integration</t>
         </is>
       </c>
-      <c r="B6" s="7" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>Einmalig</t>
         </is>
       </c>
-      <c r="C6" s="16">
-        <f>'1. Eingaben'!B15</f>
-        <v/>
-      </c>
-      <c r="D6" s="16" t="n">
+      <c r="C6" s="19">
+        <f>'1. Eingaben'!B18</f>
+        <v/>
+      </c>
+      <c r="D6" s="19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Change Management (10-15%)</t>
         </is>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>% der Basiskosten</t>
         </is>
       </c>
-      <c r="C7" s="16">
-        <f>'1. Eingaben'!B16*(C4+C5+C6)</f>
-        <v/>
-      </c>
-      <c r="D7" s="16" t="n">
+      <c r="C7" s="19">
+        <f>'1. Eingaben'!B19*(C4+C5+C6)</f>
+        <v/>
+      </c>
+      <c r="D7" s="19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="inlineStr">
+      <c r="A9" s="20" t="inlineStr">
         <is>
           <t>TOTAL KOSTEN</t>
         </is>
       </c>
-      <c r="B9" s="17" t="n"/>
-      <c r="C9" s="18">
+      <c r="B9" s="20" t="n"/>
+      <c r="C9" s="21">
         <f>SUM(C4:C7)</f>
         <v/>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="21">
         <f>SUM(D4:D7)</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>KOSTENAUFSCHLÜSSELUNG</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="n"/>
+      <c r="C11" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Anteil Training an Gesamtkosten Jahr 1</t>
         </is>
       </c>
-      <c r="C11" s="11">
+      <c r="C12" s="14">
         <f>C5/C9</f>
         <v/>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="7" t="inlineStr">
-        <is>
-          <t>Change Management Betrag</t>
-        </is>
-      </c>
-      <c r="C12" s="19">
-        <f>C7</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="14" t="inlineStr">
-        <is>
-          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot</t>
+    <row r="13">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>Kosten pro Nutzer Jahr 1</t>
+        </is>
+      </c>
+      <c r="C13" s="22">
+        <f>C9/'1. Eingaben'!B12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="17" t="inlineStr">
+        <is>
+          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot | Datenquellen: Forrester TEI, Microsoft Work Trend Index</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1201,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1209,16 +1248,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="38" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="inlineStr">
-        <is>
-          <t>NUTZENBERECHNUNG</t>
+      <c r="A1" s="18" t="inlineStr">
+        <is>
+          <t>NUTZENBERECHNUNG (BASIEREND AUF FORRESTER TEI)</t>
         </is>
       </c>
     </row>
@@ -1233,258 +1272,321 @@
       <c r="D3" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="inlineStr">
-        <is>
-          <t>Arbeitszeit pro Nutzer/Jahr (Stunden)</t>
-        </is>
-      </c>
-      <c r="B5" s="20">
-        <f>'1. Eingaben'!B9*'1. Eingaben'!B10</f>
-        <v/>
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>Zeitersparnis pro Nutzer/Monat (Forrester)</t>
+        </is>
+      </c>
+      <c r="B5" s="23">
+        <f>'1. Eingaben'!B33</f>
+        <v/>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>Stunden</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="inlineStr">
-        <is>
-          <t>Gesamtarbeitszeit alle Nutzer (Stunden)</t>
-        </is>
-      </c>
-      <c r="B6" s="20">
-        <f>B5*'1. Eingaben'!B7</f>
-        <v/>
-      </c>
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>Stundensatz</t>
+        </is>
+      </c>
+      <c r="B6" s="22">
+        <f>'1. Eingaben'!B13</f>
+        <v/>
+      </c>
+      <c r="C6" s="10" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
-        <is>
-          <t>Stundensatz</t>
-        </is>
-      </c>
-      <c r="B7" s="19">
-        <f>'1. Eingaben'!B8</f>
-        <v/>
-      </c>
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>Adoption-Rate (aus Training)</t>
+        </is>
+      </c>
+      <c r="B7" s="14">
+        <f>'1. Eingaben'!B24</f>
+        <v/>
+      </c>
+      <c r="C7" s="10" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="inlineStr">
-        <is>
-          <t>Adoption-Rate (aus Training)</t>
-        </is>
-      </c>
-      <c r="B8" s="11">
-        <f>'1. Eingaben'!B21</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="inlineStr">
-        <is>
-          <t>Zeitersparnis pro aktivem Nutzer</t>
-        </is>
-      </c>
-      <c r="B9" s="11">
-        <f>'1. Eingaben'!B30</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>Anzahl Nutzer</t>
+        </is>
+      </c>
+      <c r="B8" s="23">
+        <f>'1. Eingaben'!B12</f>
+        <v/>
+      </c>
+      <c r="C8" s="10" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>EFFEKTIVER NUTZEN</t>
         </is>
       </c>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="4" t="n"/>
-      <c r="D11" s="5" t="n"/>
+      <c r="B10" s="4" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>Aktive Nutzer (Adoption × Gesamtnutzer)</t>
+        </is>
+      </c>
+      <c r="B12" s="24">
+        <f>B8*B7</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
-        <is>
-          <t>Aktive Nutzer (Adoption × Gesamtnutzer)</t>
-        </is>
-      </c>
-      <c r="B13" s="21">
-        <f>'1. Eingaben'!B7*B8</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="inlineStr">
-        <is>
-          <t>Eingesparte Stunden/Jahr</t>
-        </is>
-      </c>
-      <c r="B14" s="21">
-        <f>B13*B5*B9</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="17" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>Eingesparte Stunden/Jahr (9h × 12 Monate × Aktive)</t>
+        </is>
+      </c>
+      <c r="B13" s="24">
+        <f>B12*B5*12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="20" t="inlineStr">
         <is>
           <t>JÄHRLICHER NUTZEN (€)</t>
         </is>
       </c>
-      <c r="B16" s="18">
-        <f>B14*B7</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="B15" s="21">
+        <f>B13*B6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>Nutzen pro aktivem Nutzer/Jahr</t>
+        </is>
+      </c>
+      <c r="B17" s="22">
+        <f>B5*12*B6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>Nutzen pro aktivem Nutzer/Monat</t>
+        </is>
+      </c>
+      <c r="B18" s="22">
+        <f>B5*B6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>ROI PRO AKTIVEM NUTZER</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="5" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>Lizenzkosten pro Monat</t>
+        </is>
+      </c>
+      <c r="B22" s="22">
+        <f>'1. Eingaben'!B17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>Nutzen pro Monat (9h × Stundensatz)</t>
+        </is>
+      </c>
+      <c r="B23" s="22">
+        <f>B18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>ROI pro aktivem Nutzer</t>
+        </is>
+      </c>
+      <c r="B24" s="25">
+        <f>(B23-B22)/B22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>EINFLUSS DER ADOPTION-RATE</t>
         </is>
       </c>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="5" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="inlineStr">
+      <c r="B27" s="4" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="5" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="9" t="inlineStr">
         <is>
           <t>Training-Budget</t>
         </is>
       </c>
-      <c r="B20" s="6" t="inlineStr">
+      <c r="B28" s="9" t="inlineStr">
         <is>
           <t>Adoption</t>
         </is>
       </c>
-      <c r="C20" s="6" t="inlineStr">
+      <c r="C28" s="9" t="inlineStr">
         <is>
           <t>Jährlicher Nutzen</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
+      <c r="D28" s="9" t="inlineStr">
         <is>
           <t>Delta zu aktuell</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="7" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="10" t="inlineStr">
         <is>
           <t>Kein Training (€0)</t>
         </is>
       </c>
-      <c r="B21" s="22">
+      <c r="B29" s="26">
         <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-0/600))))</f>
         <v/>
       </c>
-      <c r="C21" s="16">
-        <f>B21*'1. Eingaben'!B7*'3. Nutzen'!B5*'1. Eingaben'!B30*'1. Eingaben'!B8</f>
-        <v/>
-      </c>
-      <c r="D21" s="23">
-        <f>C21-$B$16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="inlineStr">
+      <c r="C29" s="19">
+        <f>B29*'1. Eingaben'!B12*'1. Eingaben'!B33*12*'1. Eingaben'!B13</f>
+        <v/>
+      </c>
+      <c r="D29" s="27">
+        <f>C29-$B$15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="inlineStr">
         <is>
           <t>Basis (€300)</t>
         </is>
       </c>
-      <c r="B22" s="22">
+      <c r="B30" s="26">
         <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-300/600))))</f>
         <v/>
       </c>
-      <c r="C22" s="16">
-        <f>B22*'1. Eingaben'!B7*'3. Nutzen'!B5*'1. Eingaben'!B30*'1. Eingaben'!B8</f>
-        <v/>
-      </c>
-      <c r="D22" s="23">
-        <f>C22-$B$16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="C30" s="19">
+        <f>B30*'1. Eingaben'!B12*'1. Eingaben'!B33*12*'1. Eingaben'!B13</f>
+        <v/>
+      </c>
+      <c r="D30" s="27">
+        <f>C30-$B$15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="10" t="inlineStr">
         <is>
           <t>Standard (€800)</t>
         </is>
       </c>
-      <c r="B23" s="22">
+      <c r="B31" s="26">
         <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-800/600))))</f>
         <v/>
       </c>
-      <c r="C23" s="16">
-        <f>B23*'1. Eingaben'!B7*'3. Nutzen'!B5*'1. Eingaben'!B30*'1. Eingaben'!B8</f>
-        <v/>
-      </c>
-      <c r="D23" s="23">
-        <f>C23-$B$16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="7" t="inlineStr">
+      <c r="C31" s="19">
+        <f>B31*'1. Eingaben'!B12*'1. Eingaben'!B33*12*'1. Eingaben'!B13</f>
+        <v/>
+      </c>
+      <c r="D31" s="27">
+        <f>C31-$B$15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="inlineStr">
         <is>
           <t>Professional (€1.500)</t>
         </is>
       </c>
-      <c r="B24" s="22">
+      <c r="B32" s="26">
         <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-1500/600))))</f>
         <v/>
       </c>
-      <c r="C24" s="16">
-        <f>B24*'1. Eingaben'!B7*'3. Nutzen'!B5*'1. Eingaben'!B30*'1. Eingaben'!B8</f>
-        <v/>
-      </c>
-      <c r="D24" s="23">
-        <f>C24-$B$16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="7" t="inlineStr">
+      <c r="C32" s="19">
+        <f>B32*'1. Eingaben'!B12*'1. Eingaben'!B33*12*'1. Eingaben'!B13</f>
+        <v/>
+      </c>
+      <c r="D32" s="27">
+        <f>C32-$B$15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="inlineStr">
         <is>
           <t>Premium (€2.500)</t>
         </is>
       </c>
-      <c r="B25" s="22">
+      <c r="B33" s="26">
         <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-2500/600))))</f>
         <v/>
       </c>
-      <c r="C25" s="16">
-        <f>B25*'1. Eingaben'!B7*'3. Nutzen'!B5*'1. Eingaben'!B30*'1. Eingaben'!B8</f>
-        <v/>
-      </c>
-      <c r="D25" s="23">
-        <f>C25-$B$16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="17" t="inlineStr">
+      <c r="C33" s="19">
+        <f>B33*'1. Eingaben'!B12*'1. Eingaben'!B33*12*'1. Eingaben'!B13</f>
+        <v/>
+      </c>
+      <c r="D33" s="27">
+        <f>C33-$B$15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="20" t="inlineStr">
         <is>
           <t>→ Ihre aktuelle Auswahl</t>
         </is>
       </c>
-      <c r="B27" s="24">
-        <f>'1. Eingaben'!B21</f>
-        <v/>
-      </c>
-      <c r="C27" s="18">
-        <f>B16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="14" t="inlineStr">
-        <is>
-          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot</t>
+      <c r="B35" s="25">
+        <f>'1. Eingaben'!B24</f>
+        <v/>
+      </c>
+      <c r="C35" s="21">
+        <f>B15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="17" t="inlineStr">
+        <is>
+          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot | Datenquellen: Forrester TEI, Microsoft Work Trend Index</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A10:D10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1496,7 +1598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1504,9 +1606,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -1514,376 +1616,395 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>ROI-DASHBOARD</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>Berechnungsbasis: Forrester TEI Study (9h/Monat) + Microsoft Work Trend Index (77% Produktivität)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>SCHLÜSSELKENNZAHLEN</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n"/>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="5" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="5" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Investition Jahr 1</t>
         </is>
       </c>
-      <c r="B5" s="18">
+      <c r="B7" s="21">
         <f>'2. Kosten'!C9</f>
         <v/>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Jährlicher Nutzen</t>
         </is>
       </c>
-      <c r="B6" s="18">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="B8" s="21">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>Netto-Nutzen Jahr 1</t>
         </is>
       </c>
-      <c r="B7" s="18">
-        <f>'3. Nutzen'!B16-'2. Kosten'!C9</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="B9" s="21">
+        <f>'3. Nutzen'!B15-'2. Kosten'!C9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>ROI Jahr 1</t>
         </is>
       </c>
-      <c r="B8" s="24">
-        <f>('3. Nutzen'!B16-'2. Kosten'!C9)/'2. Kosten'!C9</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="B10" s="25">
+        <f>('3. Nutzen'!B15-'2. Kosten'!C9)/'2. Kosten'!C9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>Break-even (Monate)</t>
         </is>
       </c>
-      <c r="B9" s="25">
-        <f>'2. Kosten'!C9/('3. Nutzen'!B16/12)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="B11" s="28">
+        <f>'2. Kosten'!C9/('3. Nutzen'!B15/12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Adoption-Rate</t>
         </is>
       </c>
-      <c r="B10" s="24">
-        <f>'1. Eingaben'!B21</f>
+      <c r="B12" s="25">
+        <f>'1. Eingaben'!B24</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>ROI pro aktivem Nutzer</t>
+        </is>
+      </c>
+      <c r="B13" s="25">
+        <f>'3. Nutzen'!B24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>5-JAHRES-PROGNOSE</t>
         </is>
       </c>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" s="4" t="n"/>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="5" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="inlineStr"/>
-      <c r="B14" s="6" t="inlineStr">
+      <c r="B16" s="4" t="n"/>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="4" t="n"/>
+      <c r="E16" s="4" t="n"/>
+      <c r="F16" s="4" t="n"/>
+      <c r="G16" s="5" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="9" t="inlineStr"/>
+      <c r="B17" s="9" t="inlineStr">
         <is>
           <t>Jahr 1</t>
         </is>
       </c>
-      <c r="C14" s="6" t="inlineStr">
+      <c r="C17" s="9" t="inlineStr">
         <is>
           <t>Jahr 2</t>
         </is>
       </c>
-      <c r="D14" s="6" t="inlineStr">
+      <c r="D17" s="9" t="inlineStr">
         <is>
           <t>Jahr 3</t>
         </is>
       </c>
-      <c r="E14" s="6" t="inlineStr">
+      <c r="E17" s="9" t="inlineStr">
         <is>
           <t>Jahr 4</t>
         </is>
       </c>
-      <c r="F14" s="6" t="inlineStr">
+      <c r="F17" s="9" t="inlineStr">
         <is>
           <t>Jahr 5</t>
         </is>
       </c>
-      <c r="G14" s="6" t="inlineStr">
+      <c r="G17" s="9" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>Kosten</t>
         </is>
       </c>
-      <c r="B15" s="16">
+      <c r="B18" s="19">
         <f>'2. Kosten'!C9</f>
         <v/>
       </c>
-      <c r="C15" s="16">
+      <c r="C18" s="19">
         <f>'2. Kosten'!D9</f>
         <v/>
       </c>
-      <c r="D15" s="16">
+      <c r="D18" s="19">
         <f>'2. Kosten'!D9</f>
         <v/>
       </c>
-      <c r="E15" s="16">
+      <c r="E18" s="19">
         <f>'2. Kosten'!D9</f>
         <v/>
       </c>
-      <c r="F15" s="16">
+      <c r="F18" s="19">
         <f>'2. Kosten'!D9</f>
         <v/>
       </c>
-      <c r="G15" s="16">
-        <f>SUM(B15:F15)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="inlineStr">
+      <c r="G18" s="19">
+        <f>SUM(B18:F18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>Nutzen</t>
         </is>
       </c>
-      <c r="B16" s="16">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-      <c r="C16" s="16">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-      <c r="D16" s="16">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-      <c r="E16" s="16">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-      <c r="F16" s="16">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-      <c r="G16" s="16">
-        <f>SUM(B16:F16)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="B19" s="19">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+      <c r="C19" s="19">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+      <c r="D19" s="19">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+      <c r="E19" s="19">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+      <c r="F19" s="19">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+      <c r="G19" s="19">
+        <f>SUM(B19:F19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>Netto-Nutzen</t>
         </is>
       </c>
-      <c r="B17" s="16">
-        <f>B16-B15</f>
-        <v/>
-      </c>
-      <c r="C17" s="16">
-        <f>C16-C15</f>
-        <v/>
-      </c>
-      <c r="D17" s="16">
-        <f>D16-D15</f>
-        <v/>
-      </c>
-      <c r="E17" s="16">
-        <f>E16-E15</f>
-        <v/>
-      </c>
-      <c r="F17" s="16">
-        <f>F16-F15</f>
-        <v/>
-      </c>
-      <c r="G17" s="16">
-        <f>SUM(B17:F17)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="26" t="inlineStr">
+      <c r="B20" s="19">
+        <f>B19-B18</f>
+        <v/>
+      </c>
+      <c r="C20" s="19">
+        <f>C19-C18</f>
+        <v/>
+      </c>
+      <c r="D20" s="19">
+        <f>D19-D18</f>
+        <v/>
+      </c>
+      <c r="E20" s="19">
+        <f>E19-E18</f>
+        <v/>
+      </c>
+      <c r="F20" s="19">
+        <f>F19-F18</f>
+        <v/>
+      </c>
+      <c r="G20" s="19">
+        <f>SUM(B20:F20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="29" t="inlineStr">
         <is>
           <t>Kumuliert</t>
         </is>
       </c>
-      <c r="B18" s="27">
-        <f>B17</f>
-        <v/>
-      </c>
-      <c r="C18" s="27">
-        <f>B18+C17</f>
-        <v/>
-      </c>
-      <c r="D18" s="27">
-        <f>C18+D17</f>
-        <v/>
-      </c>
-      <c r="E18" s="27">
-        <f>D18+E17</f>
-        <v/>
-      </c>
-      <c r="F18" s="27">
-        <f>E18+F17</f>
-        <v/>
-      </c>
-      <c r="G18" s="27">
-        <f>F18</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>EINFLUSS DES TRAININGS AUF DEN ROI</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="5" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="inlineStr">
-        <is>
-          <t>Ihr Training-Budget:</t>
-        </is>
-      </c>
-      <c r="B23" s="18">
-        <f>'1. Eingaben'!B20</f>
-        <v/>
-      </c>
-      <c r="C23" s="7" t="inlineStr">
+      <c r="B21" s="30">
+        <f>B20</f>
+        <v/>
+      </c>
+      <c r="C21" s="30">
+        <f>B21+C20</f>
+        <v/>
+      </c>
+      <c r="D21" s="30">
+        <f>C21+D20</f>
+        <v/>
+      </c>
+      <c r="E21" s="30">
+        <f>D21+E20</f>
+        <v/>
+      </c>
+      <c r="F21" s="30">
+        <f>E21+F20</f>
+        <v/>
+      </c>
+      <c r="G21" s="30">
+        <f>F21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>WERT DES TRAININGS</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="n"/>
+      <c r="C24" s="4" t="n"/>
+      <c r="D24" s="4" t="n"/>
+      <c r="E24" s="4" t="n"/>
+      <c r="F24" s="5" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="inlineStr">
+        <is>
+          <t>Training-Budget:</t>
+        </is>
+      </c>
+      <c r="B26" s="21">
+        <f>'1. Eingaben'!B23</f>
+        <v/>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
         <is>
           <t>pro Mitarbeiter</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="7" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="10" t="inlineStr">
         <is>
           <t>Resultierende Adoption:</t>
         </is>
       </c>
-      <c r="B24" s="24">
-        <f>'1. Eingaben'!B21</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="inlineStr">
-        <is>
-          <t>Ohne Training (€0):</t>
-        </is>
-      </c>
-      <c r="B26" s="22">
-        <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-0/600))))</f>
-        <v/>
-      </c>
-      <c r="C26" s="7" t="inlineStr">
+      <c r="B27" s="25">
+        <f>'1. Eingaben'!B24</f>
+        <v/>
+      </c>
+      <c r="C27" s="31" t="inlineStr">
+        <is>
+          <t>(77% berichten höhere Produktivität)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="inlineStr">
+        <is>
+          <t>Szenario OHNE Training:</t>
+        </is>
+      </c>
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="C29" s="10" t="inlineStr">
         <is>
           <t>Adoption</t>
         </is>
       </c>
-      <c r="D26" s="16">
-        <f>B26*'1. Eingaben'!B7*'3. Nutzen'!B5*'1. Eingaben'!B30*'1. Eingaben'!B8-'2. Kosten'!C9+'1. Eingaben'!B7*'1. Eingaben'!B20</f>
-        <v/>
-      </c>
-      <c r="E26" s="7" t="inlineStr">
+      <c r="D29" s="19">
+        <f>0.05*'1. Eingaben'!B12*'1. Eingaben'!B33*12*'1. Eingaben'!B13-'2. Kosten'!C9+'1. Eingaben'!B12*'1. Eingaben'!B23</f>
+        <v/>
+      </c>
+      <c r="E29" s="10" t="inlineStr">
         <is>
           <t>Netto-Nutzen Jahr 1</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="7" t="inlineStr">
-        <is>
-          <t>Mit Ihrem Budget:</t>
-        </is>
-      </c>
-      <c r="B27" s="24">
-        <f>'1. Eingaben'!B21</f>
-        <v/>
-      </c>
-      <c r="C27" s="7" t="inlineStr">
+    <row r="30">
+      <c r="A30" s="10" t="inlineStr">
+        <is>
+          <t>Szenario MIT Training:</t>
+        </is>
+      </c>
+      <c r="B30" s="25">
+        <f>'1. Eingaben'!B24</f>
+        <v/>
+      </c>
+      <c r="C30" s="10" t="inlineStr">
         <is>
           <t>Adoption</t>
         </is>
       </c>
-      <c r="D27" s="18">
-        <f>'3. Nutzen'!B16-'2. Kosten'!C9</f>
-        <v/>
-      </c>
-      <c r="E27" s="7" t="inlineStr">
+      <c r="D30" s="21">
+        <f>'3. Nutzen'!B15-'2. Kosten'!C9</f>
+        <v/>
+      </c>
+      <c r="E30" s="10" t="inlineStr">
         <is>
           <t>Netto-Nutzen Jahr 1</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="28" t="inlineStr">
-        <is>
-          <t>Mehrwert durch Training:</t>
-        </is>
-      </c>
-      <c r="D29" s="29">
-        <f>D27-D26</f>
-        <v/>
-      </c>
-      <c r="E29" s="7" t="inlineStr">
-        <is>
-          <t>zusätzlicher Nutzen</t>
-        </is>
-      </c>
-    </row>
     <row r="32">
-      <c r="A32" s="14" t="inlineStr">
-        <is>
-          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot</t>
+      <c r="A32" s="32" t="inlineStr">
+        <is>
+          <t>MEHRWERT DURCH TRAINING:</t>
+        </is>
+      </c>
+      <c r="D32" s="33">
+        <f>D30-D29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="17" t="inlineStr">
+        <is>
+          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot | Datenquellen: Forrester TEI, Microsoft Work Trend Index</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A16:G16"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1895,7 +2016,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1903,195 +2024,220 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="45" customWidth="1" min="1" max="1"/>
+    <col width="55" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="30" t="inlineStr">
+      <c r="A1" s="34" t="inlineStr">
         <is>
           <t>EXECUTIVE SUMMARY</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>Basierend auf: Forrester TEI Study &amp; Microsoft Work Trend Index</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>INVESTITIONSÜBERSICHT</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n"/>
-      <c r="C3" s="5" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="5" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Anzahl Copilot-Nutzer</t>
         </is>
       </c>
-      <c r="B5" s="31">
-        <f>'1. Eingaben'!B7</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="inlineStr">
+      <c r="B7" s="35">
+        <f>'1. Eingaben'!B12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Training-Budget pro MA</t>
         </is>
       </c>
-      <c r="B6" s="18">
-        <f>'1. Eingaben'!B20</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="B8" s="21">
+        <f>'1. Eingaben'!B23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>Erwartete Adoption-Rate</t>
         </is>
       </c>
-      <c r="B7" s="24">
-        <f>'1. Eingaben'!B21</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="B9" s="25">
+        <f>'1. Eingaben'!B24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>Zeitersparnis/Nutzer/Monat</t>
+        </is>
+      </c>
+      <c r="B10" s="36">
+        <f>'1. Eingaben'!B33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>Investition Jahr 1</t>
         </is>
       </c>
-      <c r="B8" s="18">
+      <c r="B11" s="21">
         <f>'2. Kosten'!C9</f>
         <v/>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="7" t="inlineStr">
-        <is>
-          <t>Jährliche Folgekosten</t>
-        </is>
-      </c>
-      <c r="B9" s="18">
-        <f>'2. Kosten'!D9</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>ERGEBNIS</t>
         </is>
       </c>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="5" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="inlineStr">
-        <is>
-          <t>Erwarteter Nutzen (Jahr 1)</t>
-        </is>
-      </c>
-      <c r="B14" s="18">
-        <f>'3. Nutzen'!B16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+      <c r="B14" s="4" t="n"/>
+      <c r="C14" s="5" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>Jährlicher Nutzen</t>
+        </is>
+      </c>
+      <c r="B16" s="21">
+        <f>'3. Nutzen'!B15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>ROI Jahr 1</t>
         </is>
       </c>
-      <c r="B15" s="24">
-        <f>'4. ROI-Dashboard'!B8</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="inlineStr">
+      <c r="B17" s="25">
+        <f>'4. ROI-Dashboard'!B10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>Break-even (Monate)</t>
         </is>
       </c>
-      <c r="B16" s="25">
-        <f>'4. ROI-Dashboard'!B9</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="B18" s="28">
+        <f>'4. ROI-Dashboard'!B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>ROI pro aktivem Nutzer</t>
+        </is>
+      </c>
+      <c r="B19" s="25">
+        <f>'3. Nutzen'!B24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>5-Jahres Netto-Nutzen</t>
         </is>
       </c>
-      <c r="B17" s="18">
-        <f>'4. ROI-Dashboard'!G18</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="inlineStr">
-        <is>
-          <t>WICHTIGER HINWEIS</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="5" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="32" t="inlineStr">
-        <is>
-          <t>Die Adoption-Rate ist der entscheidende Faktor für den ROI.</t>
-        </is>
+      <c r="B20" s="21">
+        <f>'4. ROI-Dashboard'!G21</f>
+        <v/>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Ohne angemessenes Training nutzen erfahrungsgemäß nur 5-15%</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>der Mitarbeiter Copilot regelmäßig – die Investition verpufft.</t>
-        </is>
-      </c>
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>ERKENNTNISSE AUS DEN STUDIEN</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="n"/>
+      <c r="C23" s="5" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" s="37" t="inlineStr">
+        <is>
+          <t>▸ Forrester TEI Study: 9 Stunden Zeitersparnis pro Nutzer/Monat</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Mit professionellem Training erreichen Sie 60-85% aktive Nutzung</t>
+      <c r="A26" s="37" t="inlineStr">
+        <is>
+          <t>▸ Microsoft Work Trend Index: 77% der trainierten Nutzer berichten</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>und realisieren den vollen Produktivitätsgewinn.</t>
+      <c r="A27" s="37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   höhere Produktivität</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="37" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="37" t="inlineStr">
+        <is>
+          <t>▸ Die Adoption-Rate ist der entscheidende Erfolgsfaktor</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="14" t="inlineStr">
-        <is>
-          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot</t>
+      <c r="A30" s="37" t="inlineStr">
+        <is>
+          <t>▸ Ohne Training: nur 5-15% aktive Nutzung</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="37" t="inlineStr">
+        <is>
+          <t>▸ Mit professionellem Training: 60-85% aktive Nutzung</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="17" t="inlineStr">
+        <is>
+          <t>© copilotenschule.de - ROI-Rechner für Microsoft Copilot | Datenquellen: Forrester TEI, Microsoft Work Trend Index</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: ROI-Rechner Standardwerte aktualisiert
Artikel (CopilotRoiBerechnen.tsx):
- Training-Kosten: €800 → €1.000 pro Mitarbeiter
- Zeitersparnis: 30% → 9h/Monat (≈ 5,2% bei 40h/Woche Vollzeit)
- Beispielrechnung neu kalkuliert (ROI 288% statt 2.191%)
- Forrester-Praxisbeispiel inkl. Trainingskosten (ROI 297%)
- Annahmen explizit dokumentiert

Excel (Copilot-ROI-Rechner.xlsx):
- Training-Budget Default: €800 → €1.000
- Hinweistexte aktualisiert (Standard €1.000)
- Zeitersparnis-Hinweis: 9h/Monat ≈ 5,2% bei 40h/Woche

Quellen: Forrester TEI Study, Microsoft Work Trend Index

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/downloads/Copilot-ROI-Rechner.xlsx
+++ b/public/downloads/Copilot-ROI-Rechner.xlsx
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="B23" s="11" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="C23" s="10" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
       </c>
       <c r="D23" s="10" t="inlineStr">
         <is>
-          <t>Empfohlen: €500-1.500</t>
+          <t>Empfohlen: €800-1.500 (Standard: €1.000)</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
     <row r="29">
       <c r="A29" s="16" t="inlineStr">
         <is>
-          <t>Mit professionellem Training (€800-1.500/MA) erreichen Sie 60-85% Adoption.</t>
+          <t>Mit professionellem Training (ab €1.000/MA) erreichen Sie 60-85% Adoption.</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="D33" s="10" t="inlineStr">
         <is>
-          <t>Forrester TEI: 9h/Monat</t>
+          <t>Forrester TEI: 9h/Monat (≈ 5,2% bei 40h/Woche)</t>
         </is>
       </c>
     </row>
@@ -1036,8 +1036,8 @@
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A31:E31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1504,11 +1504,11 @@
     <row r="31">
       <c r="A31" s="10" t="inlineStr">
         <is>
-          <t>Standard (€800)</t>
+          <t>Standard (€1.000)</t>
         </is>
       </c>
       <c r="B31" s="26">
-        <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-800/600))))</f>
+        <f>MIN(0.9,MAX(0.05, 0.05 + 0.85 * (1 - EXP(-1000/600))))</f>
         <v/>
       </c>
       <c r="C31" s="19">

</xml_diff>